<commit_message>
Actualización 10 de Mayo
</commit_message>
<xml_diff>
--- a/Totales Docentes.xlsx
+++ b/Totales Docentes.xlsx
@@ -596,16 +596,16 @@
         <v>102</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>26.47</v>
+        <v>23.53</v>
       </c>
       <c r="E2">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F2">
-        <v>73.53</v>
+        <v>76.47</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -614,7 +614,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>8.800000000000001</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -625,16 +625,16 @@
         <v>145</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>10.34</v>
+        <v>9.66</v>
       </c>
       <c r="E3">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F3">
-        <v>89.66</v>
+        <v>90.34</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -741,16 +741,16 @@
         <v>118</v>
       </c>
       <c r="C7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7">
-        <v>32.2</v>
+        <v>30.51</v>
       </c>
       <c r="E7">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F7">
-        <v>67.8</v>
+        <v>69.48999999999999</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -799,25 +799,25 @@
         <v>97</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>20.62</v>
+        <v>1.03</v>
       </c>
       <c r="E9">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F9">
-        <v>79.38</v>
+        <v>83.51000000000001</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>15.46</v>
       </c>
       <c r="I9">
-        <v>8.199999999999999</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -828,25 +828,25 @@
         <v>151</v>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>26.49</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F10">
-        <v>60.93</v>
+        <v>72.84999999999999</v>
       </c>
       <c r="G10">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="H10">
-        <v>12.58</v>
+        <v>27.15</v>
       </c>
       <c r="I10">
-        <v>7.2</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -857,16 +857,16 @@
         <v>39</v>
       </c>
       <c r="C11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>28.21</v>
+        <v>25.64</v>
       </c>
       <c r="E11">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11">
-        <v>71.79000000000001</v>
+        <v>74.36</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -875,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -886,16 +886,16 @@
         <v>71</v>
       </c>
       <c r="C12">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>18.31</v>
+        <v>12.68</v>
       </c>
       <c r="E12">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F12">
-        <v>81.69</v>
+        <v>87.31999999999999</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -904,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -915,25 +915,25 @@
         <v>122</v>
       </c>
       <c r="C13">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>55.74</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F13">
-        <v>44.26</v>
+        <v>49.18</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>50.82</v>
       </c>
       <c r="I13">
-        <v>7.9</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -944,10 +944,10 @@
         <v>175</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>7.43</v>
+        <v>2.29</v>
       </c>
       <c r="E14">
         <v>132</v>
@@ -956,13 +956,13 @@
         <v>75.43000000000001</v>
       </c>
       <c r="G14">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H14">
-        <v>17.14</v>
+        <v>22.29</v>
       </c>
       <c r="I14">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1002,16 +1002,16 @@
         <v>132</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>9.85</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="F16">
-        <v>90.15000000000001</v>
+        <v>100</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1020,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>8.5</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1031,25 +1031,25 @@
         <v>57</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>35.09</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F17">
-        <v>64.91</v>
+        <v>68.42</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>31.58</v>
       </c>
       <c r="I17">
-        <v>8.5</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1118,25 +1118,25 @@
         <v>251</v>
       </c>
       <c r="C20">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>22.71</v>
+        <v>7.57</v>
       </c>
       <c r="E20">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="F20">
-        <v>77.29000000000001</v>
+        <v>83.67</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>8.76</v>
       </c>
       <c r="I20">
-        <v>7.1</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1147,16 +1147,16 @@
         <v>213</v>
       </c>
       <c r="C21">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D21">
-        <v>16.9</v>
+        <v>15.49</v>
       </c>
       <c r="E21">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F21">
-        <v>81.22</v>
+        <v>82.63</v>
       </c>
       <c r="G21">
         <v>4</v>
@@ -1234,25 +1234,25 @@
         <v>78</v>
       </c>
       <c r="C24">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>32.05</v>
+        <v>10.26</v>
       </c>
       <c r="E24">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F24">
-        <v>67.95</v>
+        <v>75.64</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>14.1</v>
       </c>
       <c r="I24">
-        <v>6.8</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1292,25 +1292,25 @@
         <v>90</v>
       </c>
       <c r="C26">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>14.44</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F26">
-        <v>85.56</v>
+        <v>87.78</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>12.22</v>
       </c>
       <c r="I26">
-        <v>8.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1321,16 +1321,16 @@
         <v>116</v>
       </c>
       <c r="C27">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>34.48</v>
+        <v>32.76</v>
       </c>
       <c r="E27">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F27">
-        <v>65.52</v>
+        <v>67.23999999999999</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1339,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1350,10 +1350,10 @@
         <v>88</v>
       </c>
       <c r="C28">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D28">
-        <v>43.18</v>
+        <v>40.91</v>
       </c>
       <c r="E28">
         <v>50</v>
@@ -1362,13 +1362,13 @@
         <v>56.82</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>2.27</v>
       </c>
       <c r="I28">
-        <v>8.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1437,16 +1437,16 @@
         <v>144</v>
       </c>
       <c r="C31">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D31">
-        <v>34.72</v>
+        <v>29.17</v>
       </c>
       <c r="E31">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F31">
-        <v>65.28</v>
+        <v>70.83</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1455,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>8.4</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1582,10 +1582,10 @@
         <v>147</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>1.36</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>123</v>
@@ -1594,13 +1594,13 @@
         <v>83.67</v>
       </c>
       <c r="G36">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H36">
-        <v>14.97</v>
+        <v>16.33</v>
       </c>
       <c r="I36">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1669,25 +1669,25 @@
         <v>137</v>
       </c>
       <c r="C39">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="D39">
-        <v>54.74</v>
+        <v>17.52</v>
       </c>
       <c r="E39">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F39">
-        <v>45.26</v>
+        <v>54.01</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>28.47</v>
       </c>
       <c r="I39">
-        <v>7</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1756,10 +1756,10 @@
         <v>23</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>8.699999999999999</v>
+        <v>4.35</v>
       </c>
       <c r="E42">
         <v>19</v>
@@ -1768,13 +1768,13 @@
         <v>82.61</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H42">
-        <v>8.699999999999999</v>
+        <v>13.04</v>
       </c>
       <c r="I42">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1814,25 +1814,25 @@
         <v>96</v>
       </c>
       <c r="C44">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>31.25</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F44">
-        <v>68.75</v>
+        <v>86.45999999999999</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>13.54</v>
       </c>
       <c r="I44">
-        <v>8.699999999999999</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1872,16 +1872,16 @@
         <v>111</v>
       </c>
       <c r="C46">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D46">
-        <v>43.24</v>
+        <v>36.94</v>
       </c>
       <c r="E46">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F46">
-        <v>56.76</v>
+        <v>63.06</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -1890,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>8.199999999999999</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1901,25 +1901,25 @@
         <v>197</v>
       </c>
       <c r="C47">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D47">
-        <v>37.56</v>
+        <v>30.96</v>
       </c>
       <c r="E47">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F47">
-        <v>62.44</v>
+        <v>64.97</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>4.06</v>
       </c>
       <c r="I47">
-        <v>8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1930,16 +1930,16 @@
         <v>176</v>
       </c>
       <c r="C48">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="D48">
-        <v>50</v>
+        <v>22.16</v>
       </c>
       <c r="E48">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="F48">
-        <v>50</v>
+        <v>77.84</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1948,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>8</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1959,25 +1959,25 @@
         <v>123</v>
       </c>
       <c r="C49">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>45.53</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F49">
-        <v>54.47</v>
+        <v>59.35</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>40.65</v>
       </c>
       <c r="I49">
-        <v>8.300000000000001</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2091,22 +2091,25 @@
         <v>102</v>
       </c>
       <c r="C2">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>23.53</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>76.47</v>
       </c>
       <c r="G2">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>73.53</v>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>8.1</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2117,22 +2120,22 @@
         <v>145</v>
       </c>
       <c r="C3">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D3">
-        <v>26.21</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="F3">
-        <v>73.79000000000001</v>
+        <v>80</v>
       </c>
       <c r="G3">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H3">
-        <v>15.86</v>
+        <v>10.34</v>
       </c>
       <c r="I3">
         <v>9.6</v>
@@ -2227,25 +2230,25 @@
         <v>118</v>
       </c>
       <c r="C7">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="D7">
-        <v>81.36</v>
+        <v>53.39</v>
       </c>
       <c r="E7">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="F7">
-        <v>18.64</v>
+        <v>46.61</v>
       </c>
       <c r="G7">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="H7">
-        <v>49.15</v>
+        <v>22.88</v>
       </c>
       <c r="I7">
-        <v>8.5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2285,22 +2288,25 @@
         <v>97</v>
       </c>
       <c r="C9">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>1.03</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>74.23</v>
       </c>
       <c r="G9">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="H9">
-        <v>79.38</v>
+        <v>24.74</v>
+      </c>
+      <c r="I9">
+        <v>7.6</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2311,22 +2317,25 @@
         <v>151</v>
       </c>
       <c r="C10">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>60.93</v>
       </c>
       <c r="G10">
-        <v>111</v>
+        <v>59</v>
       </c>
       <c r="H10">
-        <v>73.51000000000001</v>
+        <v>39.07</v>
+      </c>
+      <c r="I10">
+        <v>6.7</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2337,22 +2346,25 @@
         <v>39</v>
       </c>
       <c r="C11">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>43.59</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>56.41</v>
       </c>
       <c r="G11">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="H11">
-        <v>71.79000000000001</v>
+        <v>17.95</v>
+      </c>
+      <c r="I11">
+        <v>6.9</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2363,22 +2375,25 @@
         <v>71</v>
       </c>
       <c r="C12">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>100</v>
+        <v>14.08</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>85.92</v>
       </c>
       <c r="G12">
-        <v>58</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>81.69</v>
+        <v>1.41</v>
+      </c>
+      <c r="I12">
+        <v>6.9</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2389,22 +2404,25 @@
         <v>122</v>
       </c>
       <c r="C13">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>52.46</v>
       </c>
       <c r="G13">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H13">
-        <v>44.26</v>
+        <v>47.54</v>
+      </c>
+      <c r="I13">
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2415,22 +2433,22 @@
         <v>175</v>
       </c>
       <c r="C14">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D14">
-        <v>18.29</v>
+        <v>15.43</v>
       </c>
       <c r="E14">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F14">
-        <v>70.29000000000001</v>
+        <v>72</v>
       </c>
       <c r="G14">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="H14">
-        <v>22.29</v>
+        <v>25.71</v>
       </c>
       <c r="I14">
         <v>6.8</v>
@@ -2470,22 +2488,25 @@
         <v>132</v>
       </c>
       <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>132</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>100</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
       <c r="G16">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>90.15000000000001</v>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2496,22 +2517,25 @@
         <v>57</v>
       </c>
       <c r="C17">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="D17">
-        <v>100</v>
+        <v>35.09</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>64.91</v>
       </c>
       <c r="G17">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="H17">
-        <v>64.91</v>
+        <v>35.09</v>
+      </c>
+      <c r="I17">
+        <v>8.6</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2548,22 +2572,25 @@
         <v>74</v>
       </c>
       <c r="C19">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="D19">
-        <v>100</v>
+        <v>20.27</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>79.73</v>
       </c>
       <c r="G19">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="H19">
-        <v>100</v>
+        <v>20.27</v>
+      </c>
+      <c r="I19">
+        <v>7.4</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2574,22 +2601,25 @@
         <v>251</v>
       </c>
       <c r="C20">
-        <v>251</v>
+        <v>87</v>
       </c>
       <c r="D20">
-        <v>100</v>
+        <v>34.66</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>63.75</v>
       </c>
       <c r="G20">
-        <v>194</v>
+        <v>72</v>
       </c>
       <c r="H20">
-        <v>77.29000000000001</v>
+        <v>28.69</v>
+      </c>
+      <c r="I20">
+        <v>6.9</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2600,25 +2630,25 @@
         <v>213</v>
       </c>
       <c r="C21">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D21">
-        <v>46.01</v>
+        <v>37.09</v>
       </c>
       <c r="E21">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="F21">
-        <v>53.52</v>
+        <v>62.44</v>
       </c>
       <c r="G21">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="H21">
-        <v>29.58</v>
+        <v>22.07</v>
       </c>
       <c r="I21">
-        <v>8.1</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2681,22 +2711,25 @@
         <v>78</v>
       </c>
       <c r="C24">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="D24">
-        <v>100</v>
+        <v>35.9</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>64.09999999999999</v>
       </c>
       <c r="G24">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="H24">
-        <v>67.95</v>
+        <v>25.64</v>
+      </c>
+      <c r="I24">
+        <v>7.1</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2733,22 +2766,25 @@
         <v>90</v>
       </c>
       <c r="C26">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="D26">
-        <v>100</v>
+        <v>23.33</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>73.33</v>
       </c>
       <c r="G26">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="H26">
-        <v>85.56</v>
+        <v>26.67</v>
+      </c>
+      <c r="I26">
+        <v>8.1</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2771,10 +2807,10 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H27">
-        <v>65.52</v>
+        <v>67.23999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2785,25 +2821,25 @@
         <v>88</v>
       </c>
       <c r="C28">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="D28">
-        <v>94.31999999999999</v>
+        <v>69.31999999999999</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="F28">
-        <v>5.68</v>
+        <v>30.68</v>
       </c>
       <c r="G28">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="H28">
-        <v>51.14</v>
+        <v>28.41</v>
       </c>
       <c r="I28">
-        <v>10</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2843,25 +2879,25 @@
         <v>210</v>
       </c>
       <c r="C30">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="D30">
-        <v>64.76000000000001</v>
+        <v>43.81</v>
       </c>
       <c r="E30">
-        <v>69</v>
+        <v>113</v>
       </c>
       <c r="F30">
-        <v>32.86</v>
+        <v>53.81</v>
       </c>
       <c r="G30">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="H30">
-        <v>40</v>
+        <v>19.05</v>
       </c>
       <c r="I30">
-        <v>7.6</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2872,22 +2908,25 @@
         <v>144</v>
       </c>
       <c r="C31">
-        <v>144</v>
+        <v>61</v>
       </c>
       <c r="D31">
-        <v>100</v>
+        <v>42.36</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>57.64</v>
       </c>
       <c r="G31">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="H31">
-        <v>65.28</v>
+        <v>13.19</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2898,25 +2937,25 @@
         <v>127</v>
       </c>
       <c r="C32">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="D32">
-        <v>74.02</v>
+        <v>32.28</v>
       </c>
       <c r="E32">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="F32">
-        <v>23.62</v>
+        <v>58.27</v>
       </c>
       <c r="G32">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="H32">
-        <v>76.38</v>
+        <v>41.73</v>
       </c>
       <c r="I32">
-        <v>7.9</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -3014,22 +3053,25 @@
         <v>147</v>
       </c>
       <c r="C36">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="D36">
-        <v>100</v>
+        <v>13.61</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>74.83</v>
       </c>
       <c r="G36">
-        <v>145</v>
+        <v>37</v>
       </c>
       <c r="H36">
-        <v>98.64</v>
+        <v>25.17</v>
+      </c>
+      <c r="I36">
+        <v>7.8</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -3040,22 +3082,22 @@
         <v>91</v>
       </c>
       <c r="C37">
+        <v>20</v>
+      </c>
+      <c r="D37">
+        <v>21.98</v>
+      </c>
+      <c r="E37">
+        <v>70</v>
+      </c>
+      <c r="F37">
+        <v>76.92</v>
+      </c>
+      <c r="G37">
         <v>21</v>
       </c>
-      <c r="D37">
+      <c r="H37">
         <v>23.08</v>
-      </c>
-      <c r="E37">
-        <v>69</v>
-      </c>
-      <c r="F37">
-        <v>75.81999999999999</v>
-      </c>
-      <c r="G37">
-        <v>22</v>
-      </c>
-      <c r="H37">
-        <v>24.18</v>
       </c>
       <c r="I37">
         <v>9.1</v>
@@ -3098,22 +3140,25 @@
         <v>137</v>
       </c>
       <c r="C39">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="D39">
-        <v>100</v>
+        <v>68.61</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>20.44</v>
       </c>
       <c r="G39">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="H39">
-        <v>45.26</v>
+        <v>62.04</v>
+      </c>
+      <c r="I39">
+        <v>6.4</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3124,22 +3169,25 @@
         <v>215</v>
       </c>
       <c r="C40">
-        <v>215</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>81.86</v>
       </c>
       <c r="G40">
-        <v>215</v>
+        <v>39</v>
       </c>
       <c r="H40">
-        <v>100</v>
+        <v>18.14</v>
+      </c>
+      <c r="I40">
+        <v>7.4</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3176,22 +3224,25 @@
         <v>23</v>
       </c>
       <c r="C42">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>100</v>
+        <v>4.35</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>69.56999999999999</v>
       </c>
       <c r="G42">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H42">
-        <v>91.3</v>
+        <v>26.09</v>
+      </c>
+      <c r="I42">
+        <v>6.6</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3228,22 +3279,25 @@
         <v>96</v>
       </c>
       <c r="C44">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>76.04000000000001</v>
       </c>
       <c r="G44">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="H44">
-        <v>68.75</v>
+        <v>23.96</v>
+      </c>
+      <c r="I44">
+        <v>7.4</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3254,25 +3308,25 @@
         <v>115</v>
       </c>
       <c r="C45">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>75.65000000000001</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="F45">
-        <v>24.35</v>
+        <v>100</v>
       </c>
       <c r="G45">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>75.65000000000001</v>
+        <v>0</v>
       </c>
       <c r="I45">
-        <v>9.6</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3283,22 +3337,25 @@
         <v>111</v>
       </c>
       <c r="C46">
-        <v>111</v>
+        <v>50</v>
       </c>
       <c r="D46">
-        <v>100</v>
+        <v>45.05</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>54.95</v>
       </c>
       <c r="G46">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="H46">
-        <v>56.76</v>
+        <v>8.109999999999999</v>
+      </c>
+      <c r="I46">
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -3309,22 +3366,25 @@
         <v>197</v>
       </c>
       <c r="C47">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="D47">
-        <v>100</v>
+        <v>90.86</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>9.140000000000001</v>
       </c>
       <c r="G47">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H47">
-        <v>62.44</v>
+        <v>59.9</v>
+      </c>
+      <c r="I47">
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3335,22 +3395,25 @@
         <v>176</v>
       </c>
       <c r="C48">
-        <v>176</v>
+        <v>51</v>
       </c>
       <c r="D48">
-        <v>100</v>
+        <v>28.98</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>71.02</v>
       </c>
       <c r="G48">
-        <v>88</v>
+        <v>12</v>
       </c>
       <c r="H48">
-        <v>50</v>
+        <v>6.82</v>
+      </c>
+      <c r="I48">
+        <v>7.3</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3361,25 +3424,25 @@
         <v>123</v>
       </c>
       <c r="C49">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="D49">
-        <v>86.18000000000001</v>
+        <v>57.72</v>
       </c>
       <c r="E49">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="F49">
-        <v>13.82</v>
+        <v>42.28</v>
       </c>
       <c r="G49">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="H49">
-        <v>40.65</v>
+        <v>57.72</v>
       </c>
       <c r="I49">
-        <v>9.699999999999999</v>
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3390,22 +3453,25 @@
         <v>179</v>
       </c>
       <c r="C50">
-        <v>179</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>77.65000000000001</v>
       </c>
       <c r="G50">
-        <v>179</v>
+        <v>40</v>
       </c>
       <c r="H50">
-        <v>100</v>
+        <v>22.35</v>
+      </c>
+      <c r="I50">
+        <v>7.9</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3490,16 +3556,16 @@
         <v>102</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D2">
-        <v>26.47</v>
+        <v>23.53</v>
       </c>
       <c r="E2">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F2">
-        <v>73.53</v>
+        <v>76.47</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3508,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>8.800000000000001</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3519,16 +3585,16 @@
         <v>145</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>10.34</v>
+        <v>9.66</v>
       </c>
       <c r="E3">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F3">
-        <v>89.66</v>
+        <v>90.34</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -3635,16 +3701,16 @@
         <v>118</v>
       </c>
       <c r="C7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D7">
-        <v>32.2</v>
+        <v>30.51</v>
       </c>
       <c r="E7">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F7">
-        <v>67.8</v>
+        <v>69.48999999999999</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3693,25 +3759,25 @@
         <v>97</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>20.62</v>
+        <v>1.03</v>
       </c>
       <c r="E9">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F9">
-        <v>79.38</v>
+        <v>74.23</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>24.74</v>
       </c>
       <c r="I9">
-        <v>8.199999999999999</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3722,10 +3788,10 @@
         <v>151</v>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>26.49</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>92</v>
@@ -3734,13 +3800,13 @@
         <v>60.93</v>
       </c>
       <c r="G10">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="H10">
-        <v>12.58</v>
+        <v>39.07</v>
       </c>
       <c r="I10">
-        <v>7.2</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3751,16 +3817,16 @@
         <v>39</v>
       </c>
       <c r="C11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11">
-        <v>28.21</v>
+        <v>25.64</v>
       </c>
       <c r="E11">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F11">
-        <v>71.79000000000001</v>
+        <v>74.36</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3769,7 +3835,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3780,16 +3846,16 @@
         <v>71</v>
       </c>
       <c r="C12">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>18.31</v>
+        <v>12.68</v>
       </c>
       <c r="E12">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F12">
-        <v>81.69</v>
+        <v>87.31999999999999</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -3798,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>7.9</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3809,25 +3875,25 @@
         <v>122</v>
       </c>
       <c r="C13">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>55.74</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F13">
-        <v>44.26</v>
+        <v>52.46</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>47.54</v>
       </c>
       <c r="I13">
-        <v>7.9</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3838,25 +3904,25 @@
         <v>175</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>7.43</v>
+        <v>2.29</v>
       </c>
       <c r="E14">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F14">
-        <v>72</v>
+        <v>72.56999999999999</v>
       </c>
       <c r="G14">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H14">
-        <v>20.57</v>
+        <v>25.14</v>
       </c>
       <c r="I14">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3896,16 +3962,16 @@
         <v>132</v>
       </c>
       <c r="C16">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>9.85</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="F16">
-        <v>90.15000000000001</v>
+        <v>100</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -3914,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>8.5</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -3925,25 +3991,25 @@
         <v>57</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>35.09</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F17">
-        <v>64.91</v>
+        <v>70.18000000000001</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>29.82</v>
       </c>
       <c r="I17">
-        <v>8.5</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -4012,25 +4078,25 @@
         <v>251</v>
       </c>
       <c r="C20">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>22.71</v>
+        <v>7.57</v>
       </c>
       <c r="E20">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="F20">
-        <v>77.29000000000001</v>
+        <v>83.67</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>8.76</v>
       </c>
       <c r="I20">
-        <v>7.1</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -4041,22 +4107,22 @@
         <v>213</v>
       </c>
       <c r="C21">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D21">
-        <v>16.9</v>
+        <v>15.49</v>
       </c>
       <c r="E21">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F21">
-        <v>82.16</v>
+        <v>84.04000000000001</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21">
-        <v>0.9399999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="I21">
         <v>7.2</v>
@@ -4128,25 +4194,25 @@
         <v>78</v>
       </c>
       <c r="C24">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>32.05</v>
+        <v>10.26</v>
       </c>
       <c r="E24">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F24">
-        <v>67.95</v>
+        <v>79.48999999999999</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>10.26</v>
       </c>
       <c r="I24">
-        <v>6.8</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4186,25 +4252,25 @@
         <v>90</v>
       </c>
       <c r="C26">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>14.44</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F26">
-        <v>85.56</v>
+        <v>87.78</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>12.22</v>
       </c>
       <c r="I26">
-        <v>8.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -4215,16 +4281,16 @@
         <v>116</v>
       </c>
       <c r="C27">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>34.48</v>
+        <v>32.76</v>
       </c>
       <c r="E27">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F27">
-        <v>65.52</v>
+        <v>67.23999999999999</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -4233,7 +4299,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -4244,16 +4310,16 @@
         <v>88</v>
       </c>
       <c r="C28">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D28">
-        <v>43.18</v>
+        <v>40.91</v>
       </c>
       <c r="E28">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F28">
-        <v>56.82</v>
+        <v>59.09</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -4262,7 +4328,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>8.300000000000001</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -4331,16 +4397,16 @@
         <v>144</v>
       </c>
       <c r="C31">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D31">
-        <v>34.72</v>
+        <v>29.17</v>
       </c>
       <c r="E31">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F31">
-        <v>65.28</v>
+        <v>70.83</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -4349,7 +4415,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>8.4</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -4366,16 +4432,16 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F32">
-        <v>63.78</v>
+        <v>64.56999999999999</v>
       </c>
       <c r="G32">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H32">
-        <v>36.22</v>
+        <v>35.43</v>
       </c>
       <c r="I32">
         <v>6.9</v>
@@ -4476,25 +4542,25 @@
         <v>147</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>1.36</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F36">
-        <v>83.67</v>
+        <v>85.70999999999999</v>
       </c>
       <c r="G36">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H36">
-        <v>14.97</v>
+        <v>14.29</v>
       </c>
       <c r="I36">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -4563,25 +4629,25 @@
         <v>137</v>
       </c>
       <c r="C39">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="D39">
-        <v>54.74</v>
+        <v>17.52</v>
       </c>
       <c r="E39">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F39">
-        <v>45.26</v>
+        <v>49.64</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>32.85</v>
       </c>
       <c r="I39">
-        <v>7</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -4598,16 +4664,16 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F40">
-        <v>86.98</v>
+        <v>81.86</v>
       </c>
       <c r="G40">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="H40">
-        <v>13.02</v>
+        <v>18.14</v>
       </c>
       <c r="I40">
         <v>7.6</v>
@@ -4650,25 +4716,25 @@
         <v>23</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>8.699999999999999</v>
+        <v>4.35</v>
       </c>
       <c r="E42">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F42">
-        <v>82.61</v>
+        <v>69.56999999999999</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H42">
-        <v>8.699999999999999</v>
+        <v>26.09</v>
       </c>
       <c r="I42">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -4708,25 +4774,25 @@
         <v>96</v>
       </c>
       <c r="C44">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>31.25</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F44">
-        <v>68.75</v>
+        <v>76.04000000000001</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>23.96</v>
       </c>
       <c r="I44">
-        <v>8.699999999999999</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -4766,16 +4832,16 @@
         <v>111</v>
       </c>
       <c r="C46">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D46">
-        <v>43.24</v>
+        <v>36.94</v>
       </c>
       <c r="E46">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F46">
-        <v>56.76</v>
+        <v>63.06</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -4784,7 +4850,7 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>8.199999999999999</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -4795,25 +4861,25 @@
         <v>197</v>
       </c>
       <c r="C47">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D47">
-        <v>37.56</v>
+        <v>30.96</v>
       </c>
       <c r="E47">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F47">
-        <v>62.44</v>
+        <v>64.97</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>4.06</v>
       </c>
       <c r="I47">
-        <v>8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4824,16 +4890,16 @@
         <v>176</v>
       </c>
       <c r="C48">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="D48">
-        <v>50</v>
+        <v>22.16</v>
       </c>
       <c r="E48">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="F48">
-        <v>50</v>
+        <v>77.84</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -4842,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>8</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -4853,25 +4919,25 @@
         <v>123</v>
       </c>
       <c r="C49">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>45.53</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="F49">
-        <v>54.47</v>
+        <v>61.79</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>38.21</v>
       </c>
       <c r="I49">
-        <v>8.300000000000001</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -4888,16 +4954,16 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F50">
-        <v>79.33</v>
+        <v>77.65000000000001</v>
       </c>
       <c r="G50">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H50">
-        <v>20.67</v>
+        <v>22.35</v>
       </c>
       <c r="I50">
         <v>8</v>

</xml_diff>

<commit_message>
Actualización 11 de Mayo - Mañana
</commit_message>
<xml_diff>
--- a/Totales Docentes.xlsx
+++ b/Totales Docentes.xlsx
@@ -683,16 +683,16 @@
         <v>80</v>
       </c>
       <c r="C5">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>41.25</v>
+        <v>26.25</v>
       </c>
       <c r="E5">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F5">
-        <v>58.75</v>
+        <v>73.75</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>9.1</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -799,10 +799,10 @@
         <v>97</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1.03</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>81</v>
@@ -811,13 +811,13 @@
         <v>83.51000000000001</v>
       </c>
       <c r="G9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9">
-        <v>15.46</v>
+        <v>16.49</v>
       </c>
       <c r="I9">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1060,16 +1060,16 @@
         <v>247</v>
       </c>
       <c r="C18">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D18">
-        <v>19.84</v>
+        <v>19.03</v>
       </c>
       <c r="E18">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F18">
-        <v>80.16</v>
+        <v>80.97</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1176,22 +1176,22 @@
         <v>204</v>
       </c>
       <c r="C22">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D22">
-        <v>11.76</v>
+        <v>10.29</v>
       </c>
       <c r="E22">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F22">
-        <v>65.69</v>
+        <v>66.18000000000001</v>
       </c>
       <c r="G22">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H22">
-        <v>22.55</v>
+        <v>23.53</v>
       </c>
       <c r="I22">
         <v>7.2</v>
@@ -1205,16 +1205,16 @@
         <v>113</v>
       </c>
       <c r="C23">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23">
-        <v>41.59</v>
+        <v>38.94</v>
       </c>
       <c r="E23">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F23">
-        <v>58.41</v>
+        <v>61.06</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>8.199999999999999</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1234,10 +1234,10 @@
         <v>78</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>10.26</v>
+        <v>3.85</v>
       </c>
       <c r="E24">
         <v>59</v>
@@ -1246,13 +1246,13 @@
         <v>75.64</v>
       </c>
       <c r="G24">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H24">
-        <v>14.1</v>
+        <v>20.51</v>
       </c>
       <c r="I24">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1263,16 +1263,16 @@
         <v>180</v>
       </c>
       <c r="C25">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>31.67</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="F25">
-        <v>68.33</v>
+        <v>100</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1281,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>9</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1321,16 +1321,16 @@
         <v>116</v>
       </c>
       <c r="C27">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D27">
-        <v>32.76</v>
+        <v>27.59</v>
       </c>
       <c r="E27">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F27">
-        <v>67.23999999999999</v>
+        <v>72.41</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1339,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1408,16 +1408,16 @@
         <v>210</v>
       </c>
       <c r="C30">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D30">
-        <v>27.14</v>
+        <v>24.76</v>
       </c>
       <c r="E30">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="F30">
-        <v>68.09999999999999</v>
+        <v>70.48</v>
       </c>
       <c r="G30">
         <v>10</v>
@@ -1669,10 +1669,10 @@
         <v>137</v>
       </c>
       <c r="C39">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D39">
-        <v>17.52</v>
+        <v>9.49</v>
       </c>
       <c r="E39">
         <v>74</v>
@@ -1681,13 +1681,13 @@
         <v>54.01</v>
       </c>
       <c r="G39">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H39">
-        <v>28.47</v>
+        <v>36.5</v>
       </c>
       <c r="I39">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1727,10 +1727,10 @@
         <v>115</v>
       </c>
       <c r="C41">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E41">
         <v>92</v>
@@ -1739,13 +1739,13 @@
         <v>80</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I41">
-        <v>7.3</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1785,16 +1785,16 @@
         <v>94</v>
       </c>
       <c r="C43">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>71.28</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="F43">
-        <v>28.72</v>
+        <v>100</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -1803,7 +1803,7 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>7.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1901,25 +1901,25 @@
         <v>197</v>
       </c>
       <c r="C47">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>30.96</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="F47">
-        <v>64.97</v>
+        <v>69.54000000000001</v>
       </c>
       <c r="G47">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H47">
-        <v>4.06</v>
+        <v>30.46</v>
       </c>
       <c r="I47">
-        <v>7.8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1930,16 +1930,16 @@
         <v>176</v>
       </c>
       <c r="C48">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D48">
-        <v>22.16</v>
+        <v>16.48</v>
       </c>
       <c r="E48">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="F48">
-        <v>77.84</v>
+        <v>83.52</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2149,22 +2149,25 @@
         <v>164</v>
       </c>
       <c r="C4">
-        <v>164</v>
+        <v>64</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>39.02</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>44.51</v>
       </c>
       <c r="G4">
-        <v>164</v>
+        <v>91</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>55.49</v>
+      </c>
+      <c r="I4">
+        <v>7.6</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2175,22 +2178,25 @@
         <v>80</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="G5">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="H5">
-        <v>58.75</v>
+        <v>3.75</v>
+      </c>
+      <c r="I5">
+        <v>7.8</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2288,10 +2294,10 @@
         <v>97</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1.03</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>72</v>
@@ -2300,10 +2306,10 @@
         <v>74.23</v>
       </c>
       <c r="G9">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>24.74</v>
+        <v>25.77</v>
       </c>
       <c r="I9">
         <v>7.6</v>
@@ -2346,25 +2352,25 @@
         <v>39</v>
       </c>
       <c r="C11">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11">
-        <v>43.59</v>
+        <v>41.03</v>
       </c>
       <c r="E11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F11">
-        <v>56.41</v>
+        <v>58.97</v>
       </c>
       <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>15.38</v>
+      </c>
+      <c r="I11">
         <v>7</v>
-      </c>
-      <c r="H11">
-        <v>17.95</v>
-      </c>
-      <c r="I11">
-        <v>6.9</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2546,22 +2552,25 @@
         <v>247</v>
       </c>
       <c r="C18">
-        <v>247</v>
+        <v>69</v>
       </c>
       <c r="D18">
-        <v>100</v>
+        <v>27.94</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>72.06</v>
       </c>
       <c r="G18">
-        <v>198</v>
+        <v>22</v>
       </c>
       <c r="H18">
-        <v>80.16</v>
+        <v>8.91</v>
+      </c>
+      <c r="I18">
+        <v>7.7</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2659,22 +2668,25 @@
         <v>204</v>
       </c>
       <c r="C22">
-        <v>204</v>
+        <v>65</v>
       </c>
       <c r="D22">
-        <v>100</v>
+        <v>31.86</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>64.22</v>
       </c>
       <c r="G22">
-        <v>180</v>
+        <v>52</v>
       </c>
       <c r="H22">
-        <v>88.23999999999999</v>
+        <v>25.49</v>
+      </c>
+      <c r="I22">
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2685,22 +2697,25 @@
         <v>113</v>
       </c>
       <c r="C23">
-        <v>113</v>
+        <v>68</v>
       </c>
       <c r="D23">
-        <v>100</v>
+        <v>60.18</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>39.82</v>
       </c>
       <c r="G23">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="H23">
-        <v>58.41</v>
+        <v>21.24</v>
+      </c>
+      <c r="I23">
+        <v>8.4</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2711,25 +2726,25 @@
         <v>78</v>
       </c>
       <c r="C24">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D24">
-        <v>35.9</v>
+        <v>30.77</v>
       </c>
       <c r="E24">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F24">
-        <v>64.09999999999999</v>
+        <v>69.23</v>
       </c>
       <c r="G24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H24">
-        <v>25.64</v>
+        <v>26.92</v>
       </c>
       <c r="I24">
-        <v>7.1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2740,22 +2755,25 @@
         <v>180</v>
       </c>
       <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
         <v>180</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>100</v>
       </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
       <c r="G25">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>68.33</v>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2766,25 +2784,25 @@
         <v>90</v>
       </c>
       <c r="C26">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D26">
-        <v>23.33</v>
+        <v>17.78</v>
       </c>
       <c r="E26">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F26">
-        <v>73.33</v>
+        <v>77.78</v>
       </c>
       <c r="G26">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H26">
-        <v>26.67</v>
+        <v>22.22</v>
       </c>
       <c r="I26">
-        <v>8.1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2795,22 +2813,25 @@
         <v>116</v>
       </c>
       <c r="C27">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="D27">
-        <v>100</v>
+        <v>43.97</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>56.03</v>
       </c>
       <c r="G27">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="H27">
-        <v>67.23999999999999</v>
+        <v>16.38</v>
+      </c>
+      <c r="I27">
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2879,25 +2900,25 @@
         <v>210</v>
       </c>
       <c r="C30">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D30">
-        <v>43.81</v>
+        <v>37.14</v>
       </c>
       <c r="E30">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="F30">
-        <v>53.81</v>
+        <v>60.48</v>
       </c>
       <c r="G30">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H30">
-        <v>19.05</v>
+        <v>14.76</v>
       </c>
       <c r="I30">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3140,25 +3161,25 @@
         <v>137</v>
       </c>
       <c r="C39">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="D39">
-        <v>68.61</v>
+        <v>51.09</v>
       </c>
       <c r="E39">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="F39">
-        <v>20.44</v>
+        <v>36.5</v>
       </c>
       <c r="G39">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="H39">
-        <v>62.04</v>
+        <v>54.01</v>
       </c>
       <c r="I39">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3198,22 +3219,25 @@
         <v>115</v>
       </c>
       <c r="C41">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="D41">
-        <v>100</v>
+        <v>24.35</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>55.65</v>
       </c>
       <c r="G41">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="H41">
-        <v>80</v>
+        <v>44.35</v>
+      </c>
+      <c r="I41">
+        <v>7.3</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3253,22 +3277,25 @@
         <v>94</v>
       </c>
       <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>94</v>
       </c>
-      <c r="D43">
+      <c r="F43">
         <v>100</v>
       </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
       <c r="G43">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>28.72</v>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>6.5</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3366,25 +3393,25 @@
         <v>197</v>
       </c>
       <c r="C47">
-        <v>179</v>
+        <v>87</v>
       </c>
       <c r="D47">
-        <v>90.86</v>
+        <v>44.16</v>
       </c>
       <c r="E47">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="F47">
-        <v>9.140000000000001</v>
+        <v>54.82</v>
       </c>
       <c r="G47">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="H47">
-        <v>59.9</v>
+        <v>45.18</v>
       </c>
       <c r="I47">
-        <v>8.300000000000001</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3395,25 +3422,25 @@
         <v>176</v>
       </c>
       <c r="C48">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D48">
-        <v>28.98</v>
+        <v>16.48</v>
       </c>
       <c r="E48">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="F48">
-        <v>71.02</v>
+        <v>83.52</v>
       </c>
       <c r="G48">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="H48">
-        <v>6.82</v>
+        <v>0</v>
       </c>
       <c r="I48">
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3424,22 +3451,22 @@
         <v>123</v>
       </c>
       <c r="C49">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D49">
-        <v>57.72</v>
+        <v>55.28</v>
       </c>
       <c r="E49">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F49">
-        <v>42.28</v>
+        <v>44.72</v>
       </c>
       <c r="G49">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H49">
-        <v>57.72</v>
+        <v>55.28</v>
       </c>
       <c r="I49">
         <v>8.800000000000001</v>
@@ -3620,16 +3647,16 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F4">
-        <v>69.51000000000001</v>
+        <v>70.12</v>
       </c>
       <c r="G4">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4">
-        <v>30.49</v>
+        <v>29.88</v>
       </c>
       <c r="I4">
         <v>7.8</v>
@@ -3643,16 +3670,16 @@
         <v>80</v>
       </c>
       <c r="C5">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>41.25</v>
+        <v>26.25</v>
       </c>
       <c r="E5">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F5">
-        <v>58.75</v>
+        <v>73.75</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3661,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>9.1</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3759,10 +3786,10 @@
         <v>97</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1.03</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>72</v>
@@ -3771,13 +3798,13 @@
         <v>74.23</v>
       </c>
       <c r="G9">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H9">
-        <v>24.74</v>
+        <v>25.77</v>
       </c>
       <c r="I9">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4020,16 +4047,16 @@
         <v>247</v>
       </c>
       <c r="C18">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D18">
-        <v>19.84</v>
+        <v>19.03</v>
       </c>
       <c r="E18">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F18">
-        <v>80.16</v>
+        <v>80.97</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -4136,22 +4163,22 @@
         <v>204</v>
       </c>
       <c r="C22">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D22">
-        <v>11.76</v>
+        <v>10.29</v>
       </c>
       <c r="E22">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="F22">
-        <v>65.69</v>
+        <v>71.56999999999999</v>
       </c>
       <c r="G22">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H22">
-        <v>22.55</v>
+        <v>18.14</v>
       </c>
       <c r="I22">
         <v>7.2</v>
@@ -4165,16 +4192,16 @@
         <v>113</v>
       </c>
       <c r="C23">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D23">
-        <v>41.59</v>
+        <v>38.94</v>
       </c>
       <c r="E23">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F23">
-        <v>58.41</v>
+        <v>61.06</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -4183,7 +4210,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>8.199999999999999</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -4194,10 +4221,10 @@
         <v>78</v>
       </c>
       <c r="C24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>10.26</v>
+        <v>3.85</v>
       </c>
       <c r="E24">
         <v>62</v>
@@ -4206,13 +4233,13 @@
         <v>79.48999999999999</v>
       </c>
       <c r="G24">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H24">
-        <v>10.26</v>
+        <v>16.67</v>
       </c>
       <c r="I24">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4223,16 +4250,16 @@
         <v>180</v>
       </c>
       <c r="C25">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>31.67</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>123</v>
+        <v>180</v>
       </c>
       <c r="F25">
-        <v>68.33</v>
+        <v>100</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -4241,7 +4268,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>9</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4281,16 +4308,16 @@
         <v>116</v>
       </c>
       <c r="C27">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D27">
-        <v>32.76</v>
+        <v>27.59</v>
       </c>
       <c r="E27">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F27">
-        <v>67.23999999999999</v>
+        <v>72.41</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -4299,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -4368,16 +4395,16 @@
         <v>210</v>
       </c>
       <c r="C30">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D30">
-        <v>27.14</v>
+        <v>24.76</v>
       </c>
       <c r="E30">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F30">
-        <v>67.62</v>
+        <v>70</v>
       </c>
       <c r="G30">
         <v>11</v>
@@ -4629,10 +4656,10 @@
         <v>137</v>
       </c>
       <c r="C39">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D39">
-        <v>17.52</v>
+        <v>9.49</v>
       </c>
       <c r="E39">
         <v>68</v>
@@ -4641,13 +4668,13 @@
         <v>49.64</v>
       </c>
       <c r="G39">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H39">
-        <v>32.85</v>
+        <v>40.88</v>
       </c>
       <c r="I39">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -4687,25 +4714,25 @@
         <v>115</v>
       </c>
       <c r="C41">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="F41">
-        <v>80</v>
+        <v>66.95999999999999</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>33.04</v>
       </c>
       <c r="I41">
-        <v>7.3</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -4745,16 +4772,16 @@
         <v>94</v>
       </c>
       <c r="C43">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>71.28</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="F43">
-        <v>28.72</v>
+        <v>100</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -4763,7 +4790,7 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>7.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -4861,25 +4888,25 @@
         <v>197</v>
       </c>
       <c r="C47">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>30.96</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="F47">
-        <v>64.97</v>
+        <v>70.56</v>
       </c>
       <c r="G47">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="H47">
-        <v>4.06</v>
+        <v>29.44</v>
       </c>
       <c r="I47">
-        <v>7.8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4890,16 +4917,16 @@
         <v>176</v>
       </c>
       <c r="C48">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D48">
-        <v>22.16</v>
+        <v>16.48</v>
       </c>
       <c r="E48">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="F48">
-        <v>77.84</v>
+        <v>83.52</v>
       </c>
       <c r="G48">
         <v>0</v>

</xml_diff>

<commit_message>
Estadisticos Matutinos 15 Oct
</commit_message>
<xml_diff>
--- a/Totales Docentes.xlsx
+++ b/Totales Docentes.xlsx
@@ -770,22 +770,25 @@
         <v>167</v>
       </c>
       <c r="C8">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>48.5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>51.5</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
+      </c>
+      <c r="I8">
+        <v>7.9</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -796,16 +799,16 @@
         <v>97</v>
       </c>
       <c r="C9">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="D9">
-        <v>91.75</v>
+        <v>47.42</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="F9">
-        <v>8.25</v>
+        <v>52.58</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -814,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>8.9</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -825,22 +828,25 @@
         <v>172</v>
       </c>
       <c r="C10">
-        <v>172</v>
+        <v>51</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>29.65</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>70.34999999999999</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
+      </c>
+      <c r="I10">
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -851,16 +857,16 @@
         <v>102</v>
       </c>
       <c r="C11">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>52.94</v>
+        <v>28.43</v>
       </c>
       <c r="E11">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="F11">
-        <v>47.06</v>
+        <v>71.56999999999999</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -869,7 +875,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>8.4</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -909,22 +915,25 @@
         <v>159</v>
       </c>
       <c r="C13">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>26.42</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>69.81</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>3.77</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -935,22 +944,25 @@
         <v>189</v>
       </c>
       <c r="C14">
-        <v>189</v>
+        <v>23</v>
       </c>
       <c r="D14">
-        <v>100</v>
+        <v>12.17</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>77.78</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>10.05</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -961,22 +973,25 @@
         <v>96</v>
       </c>
       <c r="C15">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>71.88</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>28.13</v>
+      </c>
+      <c r="I15">
+        <v>7.2</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -987,16 +1002,16 @@
         <v>178</v>
       </c>
       <c r="C16">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>30.9</v>
+        <v>19.66</v>
       </c>
       <c r="E16">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="F16">
-        <v>69.09999999999999</v>
+        <v>80.34</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1005,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>8.199999999999999</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1045,16 +1060,16 @@
         <v>147</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18">
-        <v>20.41</v>
+        <v>19.73</v>
       </c>
       <c r="E18">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F18">
-        <v>79.59</v>
+        <v>80.27</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1074,25 +1089,25 @@
         <v>228</v>
       </c>
       <c r="C19">
-        <v>197</v>
+        <v>21</v>
       </c>
       <c r="D19">
-        <v>86.40000000000001</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="F19">
-        <v>13.16</v>
+        <v>71.93000000000001</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="H19">
-        <v>0.44</v>
+        <v>18.86</v>
       </c>
       <c r="I19">
-        <v>8.5</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1129,22 +1144,25 @@
         <v>120</v>
       </c>
       <c r="C21">
-        <v>120</v>
+        <v>43</v>
       </c>
       <c r="D21">
-        <v>100</v>
+        <v>35.83</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>64.17</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
+      </c>
+      <c r="I21">
+        <v>8.5</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1155,22 +1173,25 @@
         <v>212</v>
       </c>
       <c r="C22">
-        <v>212</v>
+        <v>48</v>
       </c>
       <c r="D22">
-        <v>100</v>
+        <v>22.64</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>77.36</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
         <v>0</v>
+      </c>
+      <c r="I22">
+        <v>7.4</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1181,22 +1202,25 @@
         <v>195</v>
       </c>
       <c r="C23">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="D23">
-        <v>100</v>
+        <v>28.72</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>71.28</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
+      </c>
+      <c r="I23">
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1236,22 +1260,25 @@
         <v>104</v>
       </c>
       <c r="C25">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>64.42</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>35.58</v>
+      </c>
+      <c r="I25">
+        <v>6.4</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1262,22 +1289,25 @@
         <v>105</v>
       </c>
       <c r="C26">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="D26">
-        <v>100</v>
+        <v>58.1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>41.9</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
+      </c>
+      <c r="I26">
+        <v>8.6</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1317,22 +1347,25 @@
         <v>136</v>
       </c>
       <c r="C28">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="D28">
-        <v>100</v>
+        <v>25.74</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>74.26000000000001</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1372,22 +1405,25 @@
         <v>24</v>
       </c>
       <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>24</v>
       </c>
-      <c r="D30">
-        <v>100</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
       <c r="F30">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
+      </c>
+      <c r="I30">
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1398,16 +1434,16 @@
         <v>108</v>
       </c>
       <c r="C31">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="D31">
-        <v>75</v>
+        <v>29.63</v>
       </c>
       <c r="E31">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="F31">
-        <v>25</v>
+        <v>70.37</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1416,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>8.6</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1427,22 +1463,25 @@
         <v>247</v>
       </c>
       <c r="C32">
-        <v>247</v>
+        <v>102</v>
       </c>
       <c r="D32">
-        <v>100</v>
+        <v>41.3</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>58.7</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
+      </c>
+      <c r="I32">
+        <v>7.9</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1511,22 +1550,25 @@
         <v>162</v>
       </c>
       <c r="C35">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D35">
-        <v>100</v>
+        <v>88.27</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>11.73</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
+      </c>
+      <c r="I35">
+        <v>9.300000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1537,25 +1579,25 @@
         <v>142</v>
       </c>
       <c r="C36">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="D36">
-        <v>47.18</v>
+        <v>27.46</v>
       </c>
       <c r="E36">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="F36">
-        <v>52.82</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>3.52</v>
       </c>
       <c r="I36">
-        <v>8.1</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1566,22 +1608,25 @@
         <v>65</v>
       </c>
       <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
         <v>65</v>
       </c>
-      <c r="D37">
-        <v>100</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
       <c r="F37">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
         <v>0</v>
+      </c>
+      <c r="I37">
+        <v>8.1</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1621,22 +1666,25 @@
         <v>141</v>
       </c>
       <c r="C39">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="D39">
-        <v>100</v>
+        <v>68.09</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>31.91</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
         <v>0</v>
+      </c>
+      <c r="I39">
+        <v>7.9</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1647,22 +1695,25 @@
         <v>204</v>
       </c>
       <c r="C40">
-        <v>204</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>100</v>
+        <v>0.98</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>81.86</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>17.16</v>
+      </c>
+      <c r="I40">
+        <v>7.1</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1673,22 +1724,25 @@
         <v>72</v>
       </c>
       <c r="C41">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="D41">
-        <v>100</v>
+        <v>31.94</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>68.06</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
         <v>0</v>
+      </c>
+      <c r="I41">
+        <v>7.5</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1728,22 +1782,25 @@
         <v>33</v>
       </c>
       <c r="C43">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="D43">
-        <v>100</v>
+        <v>42.42</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>57.58</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
         <v>0</v>
+      </c>
+      <c r="I43">
+        <v>7.4</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1838,22 +1895,22 @@
         <v>156</v>
       </c>
       <c r="C47">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>62.82</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="F47">
-        <v>26.92</v>
+        <v>69.23</v>
       </c>
       <c r="G47">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="H47">
-        <v>10.26</v>
+        <v>30.77</v>
       </c>
       <c r="I47">
         <v>7.1</v>
@@ -1867,16 +1924,16 @@
         <v>144</v>
       </c>
       <c r="C48">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="D48">
-        <v>81.25</v>
+        <v>30.56</v>
       </c>
       <c r="E48">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="F48">
-        <v>18.75</v>
+        <v>69.44</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -1885,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>6.3</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1896,22 +1953,25 @@
         <v>124</v>
       </c>
       <c r="C49">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="D49">
-        <v>100</v>
+        <v>47.58</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>52.42</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
         <v>0</v>
+      </c>
+      <c r="I49">
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2193,10 +2253,10 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>51.5</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2219,10 +2279,10 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="H9">
-        <v>8.25</v>
+        <v>52.58</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2245,10 +2305,10 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>70.34999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2271,10 +2331,10 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="H11">
-        <v>47.06</v>
+        <v>71.56999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2323,10 +2383,10 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>73.58</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2349,10 +2409,10 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>166</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>87.83</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2375,10 +2435,10 @@
         <v>0</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2401,10 +2461,10 @@
         <v>0</v>
       </c>
       <c r="G16">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="H16">
-        <v>69.09999999999999</v>
+        <v>80.34</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2453,10 +2513,10 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H18">
-        <v>79.59</v>
+        <v>80.27</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2479,10 +2539,10 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>31</v>
+        <v>207</v>
       </c>
       <c r="H19">
-        <v>13.6</v>
+        <v>90.79000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2531,10 +2591,10 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>64.17</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2557,10 +2617,10 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>77.36</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2583,10 +2643,10 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>71.28</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2635,10 +2695,10 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2661,10 +2721,10 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>41.9</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2713,10 +2773,10 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>74.26000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2765,10 +2825,10 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2791,10 +2851,10 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="H31">
-        <v>25</v>
+        <v>70.37</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2817,10 +2877,10 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>58.7</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2895,10 +2955,10 @@
         <v>0</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>11.73</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2921,10 +2981,10 @@
         <v>0</v>
       </c>
       <c r="G36">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="H36">
-        <v>52.82</v>
+        <v>72.54000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2947,10 +3007,10 @@
         <v>0</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2999,10 +3059,10 @@
         <v>0</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>31.91</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -3025,10 +3085,10 @@
         <v>0</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>99.02</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -3051,10 +3111,10 @@
         <v>0</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>68.06</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -3103,10 +3163,10 @@
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>57.58</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -3207,10 +3267,10 @@
         <v>0</v>
       </c>
       <c r="G47">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="H47">
-        <v>37.18</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3233,10 +3293,10 @@
         <v>0</v>
       </c>
       <c r="G48">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="H48">
-        <v>18.75</v>
+        <v>69.44</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3259,10 +3319,10 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>52.42</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3544,22 +3604,25 @@
         <v>167</v>
       </c>
       <c r="C8">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>48.5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>51.5</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
+      </c>
+      <c r="I8">
+        <v>7.9</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3570,16 +3633,16 @@
         <v>97</v>
       </c>
       <c r="C9">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="D9">
-        <v>91.75</v>
+        <v>47.42</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="F9">
-        <v>8.25</v>
+        <v>52.58</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -3588,7 +3651,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>8.9</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3599,22 +3662,25 @@
         <v>172</v>
       </c>
       <c r="C10">
-        <v>172</v>
+        <v>51</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>29.65</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>70.34999999999999</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
+      </c>
+      <c r="I10">
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3625,16 +3691,16 @@
         <v>102</v>
       </c>
       <c r="C11">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>52.94</v>
+        <v>28.43</v>
       </c>
       <c r="E11">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="F11">
-        <v>47.06</v>
+        <v>71.56999999999999</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3643,7 +3709,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>8.4</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3683,22 +3749,25 @@
         <v>159</v>
       </c>
       <c r="C13">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>26.42</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>69.81</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>3.77</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3709,22 +3778,25 @@
         <v>189</v>
       </c>
       <c r="C14">
-        <v>189</v>
+        <v>23</v>
       </c>
       <c r="D14">
-        <v>100</v>
+        <v>12.17</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>77.78</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>10.05</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3735,22 +3807,25 @@
         <v>96</v>
       </c>
       <c r="C15">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>71.88</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>28.13</v>
+      </c>
+      <c r="I15">
+        <v>7.2</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3761,16 +3836,16 @@
         <v>178</v>
       </c>
       <c r="C16">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>30.9</v>
+        <v>19.66</v>
       </c>
       <c r="E16">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="F16">
-        <v>69.09999999999999</v>
+        <v>80.34</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -3779,7 +3854,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>8.199999999999999</v>
+        <v>8.300000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -3819,16 +3894,16 @@
         <v>147</v>
       </c>
       <c r="C18">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18">
-        <v>20.41</v>
+        <v>19.73</v>
       </c>
       <c r="E18">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F18">
-        <v>79.59</v>
+        <v>80.27</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -3848,25 +3923,25 @@
         <v>228</v>
       </c>
       <c r="C19">
-        <v>197</v>
+        <v>21</v>
       </c>
       <c r="D19">
-        <v>86.40000000000001</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>164</v>
       </c>
       <c r="F19">
-        <v>13.16</v>
+        <v>71.93000000000001</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="H19">
-        <v>0.44</v>
+        <v>18.86</v>
       </c>
       <c r="I19">
-        <v>8.5</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3903,22 +3978,25 @@
         <v>120</v>
       </c>
       <c r="C21">
-        <v>120</v>
+        <v>43</v>
       </c>
       <c r="D21">
-        <v>100</v>
+        <v>35.83</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>64.17</v>
       </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
+      </c>
+      <c r="I21">
+        <v>8.5</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -3929,22 +4007,25 @@
         <v>212</v>
       </c>
       <c r="C22">
-        <v>212</v>
+        <v>48</v>
       </c>
       <c r="D22">
-        <v>100</v>
+        <v>22.64</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>77.36</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
         <v>0</v>
+      </c>
+      <c r="I22">
+        <v>7.4</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3955,22 +4036,25 @@
         <v>195</v>
       </c>
       <c r="C23">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="D23">
-        <v>100</v>
+        <v>28.72</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>71.28</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
+      </c>
+      <c r="I23">
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -4010,22 +4094,25 @@
         <v>104</v>
       </c>
       <c r="C25">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>64.42</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>35.58</v>
+      </c>
+      <c r="I25">
+        <v>6.4</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4036,22 +4123,25 @@
         <v>105</v>
       </c>
       <c r="C26">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="D26">
-        <v>100</v>
+        <v>58.1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>41.9</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
+      </c>
+      <c r="I26">
+        <v>8.6</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -4091,22 +4181,25 @@
         <v>136</v>
       </c>
       <c r="C28">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="D28">
-        <v>100</v>
+        <v>25.74</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>74.26000000000001</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -4146,22 +4239,25 @@
         <v>24</v>
       </c>
       <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
         <v>24</v>
       </c>
-      <c r="D30">
-        <v>100</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
       <c r="F30">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
+      </c>
+      <c r="I30">
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -4172,16 +4268,16 @@
         <v>108</v>
       </c>
       <c r="C31">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="D31">
-        <v>75</v>
+        <v>29.63</v>
       </c>
       <c r="E31">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="F31">
-        <v>25</v>
+        <v>70.37</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -4190,7 +4286,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>8.6</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -4201,22 +4297,25 @@
         <v>247</v>
       </c>
       <c r="C32">
-        <v>247</v>
+        <v>102</v>
       </c>
       <c r="D32">
-        <v>100</v>
+        <v>41.3</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>58.7</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
         <v>0</v>
+      </c>
+      <c r="I32">
+        <v>7.9</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -4285,22 +4384,25 @@
         <v>162</v>
       </c>
       <c r="C35">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D35">
-        <v>100</v>
+        <v>88.27</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>11.73</v>
       </c>
       <c r="G35">
         <v>0</v>
       </c>
       <c r="H35">
         <v>0</v>
+      </c>
+      <c r="I35">
+        <v>9.300000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -4311,25 +4413,25 @@
         <v>142</v>
       </c>
       <c r="C36">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="D36">
-        <v>47.18</v>
+        <v>27.46</v>
       </c>
       <c r="E36">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="F36">
-        <v>52.82</v>
+        <v>69.01000000000001</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>3.52</v>
       </c>
       <c r="I36">
-        <v>8.1</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -4340,22 +4442,25 @@
         <v>65</v>
       </c>
       <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
         <v>65</v>
       </c>
-      <c r="D37">
-        <v>100</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
       <c r="F37">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G37">
         <v>0</v>
       </c>
       <c r="H37">
         <v>0</v>
+      </c>
+      <c r="I37">
+        <v>8.1</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -4395,22 +4500,25 @@
         <v>141</v>
       </c>
       <c r="C39">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="D39">
-        <v>100</v>
+        <v>68.09</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>31.91</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
         <v>0</v>
+      </c>
+      <c r="I39">
+        <v>7.9</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -4421,22 +4529,25 @@
         <v>204</v>
       </c>
       <c r="C40">
-        <v>204</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>100</v>
+        <v>0.98</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>167</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>81.86</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>17.16</v>
+      </c>
+      <c r="I40">
+        <v>7.1</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -4447,22 +4558,25 @@
         <v>72</v>
       </c>
       <c r="C41">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="D41">
-        <v>100</v>
+        <v>31.94</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>68.06</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
         <v>0</v>
+      </c>
+      <c r="I41">
+        <v>7.5</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -4502,22 +4616,25 @@
         <v>33</v>
       </c>
       <c r="C43">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="D43">
-        <v>100</v>
+        <v>42.42</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>57.58</v>
       </c>
       <c r="G43">
         <v>0</v>
       </c>
       <c r="H43">
         <v>0</v>
+      </c>
+      <c r="I43">
+        <v>7.4</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -4612,22 +4729,22 @@
         <v>156</v>
       </c>
       <c r="C47">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>62.82</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>42</v>
+        <v>108</v>
       </c>
       <c r="F47">
-        <v>26.92</v>
+        <v>69.23</v>
       </c>
       <c r="G47">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="H47">
-        <v>10.26</v>
+        <v>30.77</v>
       </c>
       <c r="I47">
         <v>7.1</v>
@@ -4641,16 +4758,16 @@
         <v>144</v>
       </c>
       <c r="C48">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="D48">
-        <v>81.25</v>
+        <v>30.56</v>
       </c>
       <c r="E48">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="F48">
-        <v>18.75</v>
+        <v>69.44</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -4659,7 +4776,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>6.3</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -4670,22 +4787,25 @@
         <v>124</v>
       </c>
       <c r="C49">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="D49">
-        <v>100</v>
+        <v>47.58</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>52.42</v>
       </c>
       <c r="G49">
         <v>0</v>
       </c>
       <c r="H49">
         <v>0</v>
+      </c>
+      <c r="I49">
+        <v>8.800000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:9">

</xml_diff>